<commit_message>
Working ESP8266 command from browser with LED
</commit_message>
<xml_diff>
--- a/mesures/mesures.xlsx
+++ b/mesures/mesures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57fa1324d67c1d81/Dev/arduino/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthieu\OneDrive\Dev\arduino\ArduinoThermostat\mesures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -230,7 +230,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="3"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -425,6 +425,51 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Feuil2!$F$2:$F$32</c:f>
@@ -492,55 +537,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>3.456629896549877E-3</c:v>
+                  <c:v>3.4656757785699178E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4577836596728067E-3</c:v>
+                  <c:v>3.4668117447200762E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4895892752351996E-3</c:v>
+                  <c:v>3.4981231656548424E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4680426859054936E-3</c:v>
+                  <c:v>3.4769121232253752E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4917644729055282E-3</c:v>
+                  <c:v>3.5002643120925193E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4980292380685394E-3</c:v>
+                  <c:v>3.5064308255360228E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4905760975410941E-3</c:v>
+                  <c:v>3.4990945439485775E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4880659189691172E-3</c:v>
+                  <c:v>3.4966236371933236E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4880169035727878E-3</c:v>
+                  <c:v>3.4965753882146879E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4849445335936131E-3</c:v>
+                  <c:v>3.4935510257823477E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.4871359562878529E-3</c:v>
+                  <c:v>3.495708212848711E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5068639220053035E-3</c:v>
+                  <c:v>3.5151264961630589E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.6313662655863429E-3</c:v>
+                  <c:v>3.6376128821351814E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.5411307098499934E-3</c:v>
+                  <c:v>3.5488490364389337E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.5102173579912173E-3</c:v>
+                  <c:v>3.5184270259680083E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.517090457415834E-3</c:v>
+                  <c:v>3.5251914496572871E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.493705420428172E-3</c:v>
+                  <c:v>3.5021748480450711E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,16 +1338,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>423862</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>366711</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>423862</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1807,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,7 +1911,7 @@
       </c>
       <c r="H2" s="2">
         <f>$L$18+$L$19*F2+$L$20*F2*F2*F2</f>
-        <v>3.456629896549877E-3</v>
+        <v>3.4656757785699178E-3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1896,7 +1941,7 @@
       </c>
       <c r="H3" s="2">
         <f t="shared" ref="H3:H18" si="2">$L$18+$L$19*F3+$L$20*F3*F3*F3</f>
-        <v>3.4577836596728067E-3</v>
+        <v>3.4668117447200762E-3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1926,7 +1971,7 @@
       </c>
       <c r="H4" s="2">
         <f t="shared" si="2"/>
-        <v>3.4895892752351996E-3</v>
+        <v>3.4981231656548424E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1956,7 +2001,7 @@
       </c>
       <c r="H5" s="2">
         <f t="shared" si="2"/>
-        <v>3.4680426859054936E-3</v>
+        <v>3.4769121232253752E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1986,7 +2031,7 @@
       </c>
       <c r="H6" s="2">
         <f t="shared" si="2"/>
-        <v>3.4917644729055282E-3</v>
+        <v>3.5002643120925193E-3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2010,7 +2055,7 @@
       </c>
       <c r="H7" s="2">
         <f t="shared" si="2"/>
-        <v>3.4980292380685394E-3</v>
+        <v>3.5064308255360228E-3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2034,7 +2079,7 @@
       </c>
       <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>3.4905760975410941E-3</v>
+        <v>3.4990945439485775E-3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2058,7 +2103,7 @@
       </c>
       <c r="H9" s="2">
         <f t="shared" si="2"/>
-        <v>3.4880659189691172E-3</v>
+        <v>3.4966236371933236E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2082,7 +2127,7 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" si="2"/>
-        <v>3.4880169035727878E-3</v>
+        <v>3.4965753882146879E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2106,7 +2151,7 @@
       </c>
       <c r="H11" s="2">
         <f t="shared" si="2"/>
-        <v>3.4849445335936131E-3</v>
+        <v>3.4935510257823477E-3</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2130,7 +2175,7 @@
       </c>
       <c r="H12" s="2">
         <f t="shared" si="2"/>
-        <v>3.4871359562878529E-3</v>
+        <v>3.495708212848711E-3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2154,7 +2199,7 @@
       </c>
       <c r="H13" s="2">
         <f t="shared" si="2"/>
-        <v>3.5068639220053035E-3</v>
+        <v>3.5151264961630589E-3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2178,7 +2223,7 @@
       </c>
       <c r="H14" s="2">
         <f t="shared" si="2"/>
-        <v>3.6313662655863429E-3</v>
+        <v>3.6376128821351814E-3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2202,7 +2247,7 @@
       </c>
       <c r="H15" s="2">
         <f t="shared" si="2"/>
-        <v>3.5411307098499934E-3</v>
+        <v>3.5488490364389337E-3</v>
       </c>
       <c r="I15" t="s">
         <v>25</v>
@@ -2229,7 +2274,7 @@
       </c>
       <c r="H16" s="2">
         <f t="shared" si="2"/>
-        <v>3.5102173579912173E-3</v>
+        <v>3.5184270259680083E-3</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2253,7 +2298,7 @@
       </c>
       <c r="H17" s="2">
         <f t="shared" si="2"/>
-        <v>3.517090457415834E-3</v>
+        <v>3.5251914496572871E-3</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2277,13 +2322,13 @@
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>3.493705420428172E-3</v>
+        <v>3.5021748480450711E-3</v>
       </c>
       <c r="K18" t="s">
         <v>29</v>
       </c>
       <c r="L18" s="1">
-        <v>4.8000000000000001E-4</v>
+        <v>5.1000000000000004E-4</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2291,7 +2336,7 @@
         <v>27</v>
       </c>
       <c r="L19" s="1">
-        <v>2.3699999999999999E-4</v>
+        <v>2.365E-4</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2299,7 +2344,7 @@
         <v>28</v>
       </c>
       <c r="L20" s="1">
-        <v>9.9E-8</v>
+        <v>8.9999999999999999E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>